<commit_message>
add update of details to final report
</commit_message>
<xml_diff>
--- a/1-Define/Poor quality cost/Project_Charter.xlsx
+++ b/1-Define/Poor quality cost/Project_Charter.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniell/Documents/LeanSS/1-Define/Poor quality cost/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E00F0CA6-4D38-0D4A-9677-CBADD47F9869}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1889C078-A7D8-BE40-845D-98268515E5FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="500" windowWidth="47900" windowHeight="26820" xr2:uid="{6D80875F-3CA6-0E4F-AA0C-63FBC5B3114F}"/>
+    <workbookView xWindow="5540" yWindow="-28300" windowWidth="44040" windowHeight="26840" xr2:uid="{6D80875F-3CA6-0E4F-AA0C-63FBC5B3114F}"/>
   </bookViews>
   <sheets>
     <sheet name="Project_Charter" sheetId="1" r:id="rId1"/>
@@ -83,10 +83,6 @@
     <t>AREA</t>
   </si>
   <si>
-    <t>MEDISA is engaged in the manufacture and 
-marketing of polystyrene vaults and polystyrene case of different densities. The plant is in San Diego, California, USA and has approximately 150 employees. MEDISA's main market is the construction industry, and its main customer is the construction company Pastora.</t>
-  </si>
-  <si>
     <t>Decrease 80% of erros in 
 final products measurements of 
 polystyrene cases</t>
@@ -140,12 +136,6 @@
     <t>Operators</t>
   </si>
   <si>
-    <t>Julio, B.</t>
-  </si>
-  <si>
-    <t>Jesus, C.</t>
-  </si>
-  <si>
     <t>Geardo, A.</t>
   </si>
   <si>
@@ -168,9 +158,6 @@
     <t>María del Rosario García</t>
   </si>
   <si>
-    <t>A savings of $16,640,856.96 per year will be realized by reducing variations in the process. Comply with best practices and avoid product quality impacts. Increase customer satisfaction.</t>
-  </si>
-  <si>
     <t xml:space="preserve">Decrease of variation in manufacturing process of polystyrene cases.  
 </t>
   </si>
@@ -181,6 +168,18 @@
   <si>
     <t>Polystyrene vaults &amp; 
 Polystyrene cases</t>
+  </si>
+  <si>
+    <t>MEDISA company has presented several non-conformities with one of its main customers, highlighting incorrect measurements in its flaghship product. Therefore, the team will seek to reduce variations in the process and improve customer satisfaction.</t>
+  </si>
+  <si>
+    <t>A savings of $545,592.96 MXN per year will be realized by reducing variations in the process. Comply with best practices and avoid product quality impacts. Increase customer satisfaction.</t>
+  </si>
+  <si>
+    <t>Mario, M.</t>
+  </si>
+  <si>
+    <t>Citlali, B.</t>
   </si>
 </sst>
 </file>
@@ -350,12 +349,6 @@
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -363,50 +356,56 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,7 +1311,7 @@
   <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="221" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1329,251 +1328,251 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
     </row>
     <row r="3" spans="2:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="B3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="12" t="s">
+      <c r="B3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="18"/>
+      <c r="D3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="E3" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="5" t="s">
-        <v>20</v>
+      <c r="E3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="2:8" ht="34" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5" t="s">
-        <v>21</v>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" s="2"/>
+      <c r="H4" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="2:8" ht="35" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="8" t="s">
+      <c r="B5" s="18"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="F5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="G5" s="4"/>
-      <c r="H5" s="5" t="s">
-        <v>27</v>
+      <c r="E5" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" s="2"/>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="16"/>
-      <c r="H6" s="16"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
     </row>
     <row r="7" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" s="16"/>
+      <c r="D7" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4" t="s">
-        <v>32</v>
+      <c r="E7" s="18"/>
+      <c r="F7" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4" t="s">
-        <v>33</v>
+      <c r="B8" s="16"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4" t="s">
-        <v>34</v>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4" t="s">
-        <v>35</v>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="2:8" ht="28" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="18" t="s">
+      <c r="B11" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="18" t="s">
+      <c r="C11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4" t="s">
-        <v>36</v>
+      <c r="E11" s="14"/>
+      <c r="F11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="19" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4" t="s">
-        <v>37</v>
+      <c r="C12" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="13"/>
+      <c r="F12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="16" t="s">
+      <c r="B13" s="16"/>
+      <c r="C13" s="16"/>
+      <c r="D13" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16" t="s">
+      <c r="E13" s="14"/>
+      <c r="F13" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="8" t="s">
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
+      <c r="D14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="16"/>
+      <c r="F14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4" t="s">
-        <v>39</v>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="2:8" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="7"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="8" t="s">
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4" t="s">
-        <v>40</v>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="2:8" ht="53" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="8" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="G16" s="4"/>
-      <c r="H16" s="21" t="s">
-        <v>38</v>
+      <c r="G16" s="2"/>
+      <c r="H16" s="4" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="F2:H2"/>
+    <mergeCell ref="B3:C5"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="D7:E10"/>
+    <mergeCell ref="B7:C10"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="F13:H13"/>
     <mergeCell ref="D14:E16"/>
     <mergeCell ref="B12:B16"/>
     <mergeCell ref="C12:C16"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="D7:E10"/>
-    <mergeCell ref="B7:C10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="F2:H2"/>
-    <mergeCell ref="B3:C5"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="D3:D4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>